<commit_message>
Import + Plot of carbon prices
</commit_message>
<xml_diff>
--- a/code/carbon_prices_062009_122019.xlsx
+++ b/code/carbon_prices_062009_122019.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gauth\Dropbox\26_Cap_Trade_Climate\C_Codes\2_Revised\A_June_Test\1_Estimation_gvAug\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gabri\Desktop\Github\GitHub\ETS_Impact_On_Unemployment\code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E02AB5E8-D68F-414E-8B7B-F30E63819F28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF74A0C4-1175-426C-9EB6-78DD8FCEA4F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="2340" windowWidth="28800" windowHeight="11295" xr2:uid="{9EEA4CBA-FAB2-8048-A218-02F4587E1B1A}"/>
+    <workbookView xWindow="1820" yWindow="1820" windowWidth="14400" windowHeight="7270" xr2:uid="{9EEA4CBA-FAB2-8048-A218-02F4587E1B1A}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -43,9 +43,6 @@
     <t>de_obs</t>
   </si>
   <si>
-    <t>2009M6</t>
-  </si>
-  <si>
     <t>pe_obs</t>
   </si>
   <si>
@@ -53,6 +50,9 @@
   </si>
   <si>
     <t>dpe_obs</t>
+  </si>
+  <si>
+    <t>dates</t>
   </si>
 </sst>
 </file>
@@ -441,20 +441,20 @@
   <dimension ref="A1:F131"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="22.375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="15.375" style="2" customWidth="1"/>
-    <col min="3" max="3" width="14.375" style="2" customWidth="1"/>
-    <col min="5" max="5" width="14.125" customWidth="1"/>
+    <col min="1" max="1" width="22.33203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="15.33203125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="14.33203125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="14.08203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="2" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" s="2" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>0</v>
@@ -463,16 +463,16 @@
         <v>1</v>
       </c>
       <c r="D1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="F1" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="8" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>39965</v>
       </c>
@@ -493,7 +493,7 @@
         <v>-10.739294888420476</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>39995</v>
       </c>
@@ -514,7 +514,7 @@
         <v>4.533385047110901</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>40026</v>
       </c>
@@ -535,7 +535,7 @@
         <v>5.8637143101667411</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>40057</v>
       </c>
@@ -556,7 +556,7 @@
         <v>-3.217210341653201</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>40087</v>
       </c>
@@ -577,7 +577,7 @@
         <v>-5.2369577566999054E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>40118</v>
       </c>
@@ -598,7 +598,7 @@
         <v>-3.8865967705989801</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>40148</v>
       </c>
@@ -619,7 +619,7 @@
         <v>-0.25747712561176261</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>40179</v>
       </c>
@@ -640,7 +640,7 @@
         <v>-4.4668322390640194</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <v>40210</v>
       </c>
@@ -661,7 +661,7 @@
         <v>-1.0239394243638134</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
         <v>40238</v>
       </c>
@@ -682,7 +682,7 @@
         <v>-0.49790230677324687</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
         <v>40269</v>
       </c>
@@ -703,7 +703,7 @@
         <v>9.8470504636487792</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
         <v>40299</v>
       </c>
@@ -724,7 +724,7 @@
         <v>6.9365840110331973</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
         <v>40330</v>
       </c>
@@ -745,7 +745,7 @@
         <v>7.2164459611409826E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" s="1">
         <v>40360</v>
       </c>
@@ -766,7 +766,7 @@
         <v>-7.8200816194373193</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" s="1">
         <v>40391</v>
       </c>
@@ -787,7 +787,7 @@
         <v>2.2726151014997975</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" s="1">
         <v>40422</v>
       </c>
@@ -808,7 +808,7 @@
         <v>4.7494721052747453</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18" s="1">
         <v>40452</v>
       </c>
@@ -829,7 +829,7 @@
         <v>-0.22336402938835401</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19" s="1">
         <v>40483</v>
       </c>
@@ -850,7 +850,7 @@
         <v>-3.0750851275040474</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20" s="1">
         <v>40513</v>
       </c>
@@ -871,7 +871,7 @@
         <v>-3.9776895338839178</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21" s="1">
         <v>40544</v>
       </c>
@@ -892,7 +892,7 @@
         <v>-0.4436688659205239</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22" s="1">
         <v>40575</v>
       </c>
@@ -913,7 +913,7 @@
         <v>2.4443938610287699</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23" s="1">
         <v>40603</v>
       </c>
@@ -934,7 +934,7 @@
         <v>7.3647425347005013</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A24" s="1">
         <v>40634</v>
       </c>
@@ -955,7 +955,7 @@
         <v>3.7988078000546177</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A25" s="1">
         <v>40664</v>
       </c>
@@ -976,7 +976,7 @@
         <v>0.76008460065534289</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26" s="1">
         <v>40695</v>
       </c>
@@ -997,7 +997,7 @@
         <v>-8.5480421264599737</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A27" s="1">
         <v>40725</v>
       </c>
@@ -1018,7 +1018,7 @@
         <v>-18.302752625893692</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A28" s="1">
         <v>40756</v>
       </c>
@@ -1039,7 +1039,7 @@
         <v>-3.5203102340103647</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A29" s="1">
         <v>40787</v>
       </c>
@@ -1060,7 +1060,7 @@
         <v>-4.1282322602977093</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A30" s="1">
         <v>40817</v>
       </c>
@@ -1081,7 +1081,7 @@
         <v>-12.616398873946553</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A31" s="1">
         <v>40848</v>
       </c>
@@ -1102,7 +1102,7 @@
         <v>-11.235446322806538</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A32" s="1">
         <v>40878</v>
       </c>
@@ -1123,7 +1123,7 @@
         <v>-22.072355548332812</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A33" s="1">
         <v>40909</v>
       </c>
@@ -1144,7 +1144,7 @@
         <v>-7.3085059349404196</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A34" s="1">
         <v>40940</v>
       </c>
@@ -1165,7 +1165,7 @@
         <v>20.074051939960459</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A35" s="1">
         <v>40969</v>
       </c>
@@ -1186,7 +1186,7 @@
         <v>-11.111149999095009</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A36" s="1">
         <v>41000</v>
       </c>
@@ -1207,7 +1207,7 @@
         <v>-9.3812908647098521</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A37" s="1">
         <v>41030</v>
       </c>
@@ -1228,7 +1228,7 @@
         <v>-4.3429868782520415</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A38" s="1">
         <v>41061</v>
       </c>
@@ -1249,7 +1249,7 @@
         <v>6.2987004189430982</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A39" s="1">
         <v>41091</v>
       </c>
@@ -1270,7 +1270,7 @@
         <v>4.2271093420553161</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A40" s="1">
         <v>41122</v>
       </c>
@@ -1291,7 +1291,7 @@
         <v>0.83283058302968738</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A41" s="1">
         <v>41153</v>
       </c>
@@ -1312,7 +1312,7 @@
         <v>2.1456064048593464</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A42" s="1">
         <v>41183</v>
       </c>
@@ -1333,7 +1333,7 @@
         <v>1.7434191727013966</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A43" s="1">
         <v>41214</v>
       </c>
@@ -1354,7 +1354,7 @@
         <v>-5.0823896158481281</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A44" s="1">
         <v>41244</v>
       </c>
@@ -1375,7 +1375,7 @@
         <v>-11.507368699704312</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A45" s="1">
         <v>41275</v>
       </c>
@@ -1396,7 +1396,7 @@
         <v>-23.704448193118441</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A46" s="1">
         <v>41306</v>
       </c>
@@ -1417,7 +1417,7 @@
         <v>-12.11492172201234</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A47" s="1">
         <v>41334</v>
       </c>
@@ -1438,7 +1438,7 @@
         <v>-11.968669582721247</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A48" s="1">
         <v>41365</v>
       </c>
@@ -1459,7 +1459,7 @@
         <v>-6.9845689051765634</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A49" s="1">
         <v>41395</v>
       </c>
@@ -1480,7 +1480,7 @@
         <v>-7.9641077651769958</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A50" s="1">
         <v>41426</v>
       </c>
@@ -1501,7 +1501,7 @@
         <v>18.276728935027286</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A51" s="1">
         <v>41456</v>
       </c>
@@ -1522,7 +1522,7 @@
         <v>-0.66464463218143055</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A52" s="1">
         <v>41487</v>
       </c>
@@ -1543,7 +1543,7 @@
         <v>4.4763544826178103</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A53" s="1">
         <v>41518</v>
       </c>
@@ -1564,7 +1564,7 @@
         <v>16.700254188072428</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A54" s="1">
         <v>41548</v>
       </c>
@@ -1585,7 +1585,7 @@
         <v>-6.6371018938908053</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A55" s="1">
         <v>41579</v>
       </c>
@@ -1606,7 +1606,7 @@
         <v>-8.0397711930225366</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A56" s="1">
         <v>41609</v>
       </c>
@@ -1627,7 +1627,7 @@
         <v>5.1431735038460342</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A57" s="1">
         <v>41640</v>
       </c>
@@ -1648,7 +1648,7 @@
         <v>4.3134346222659641</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A58" s="1">
         <v>41671</v>
       </c>
@@ -1669,7 +1669,7 @@
         <v>26.288277067403833</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A59" s="1">
         <v>41699</v>
       </c>
@@ -1690,7 +1690,7 @@
         <v>-6.6978620186121285</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A60" s="1">
         <v>41730</v>
       </c>
@@ -1711,7 +1711,7 @@
         <v>-15.832649787530389</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A61" s="1">
         <v>41760</v>
       </c>
@@ -1732,7 +1732,7 @@
         <v>-2.2459262078247373</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A62" s="1">
         <v>41791</v>
       </c>
@@ -1753,7 +1753,7 @@
         <v>8.7766623565943398</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A63" s="1">
         <v>41821</v>
       </c>
@@ -1774,7 +1774,7 @@
         <v>6.1664165861318505</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A64" s="1">
         <v>41852</v>
       </c>
@@ -1795,7 +1795,7 @@
         <v>4.5483636521030322</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A65" s="1">
         <v>41883</v>
       </c>
@@ -1816,7 +1816,7 @@
         <v>-3.7035512331356677</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A66" s="1">
         <v>41913</v>
       </c>
@@ -1837,7 +1837,7 @@
         <v>1.17761342552802</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A67" s="1">
         <v>41944</v>
       </c>
@@ -1858,7 +1858,7 @@
         <v>11.862301940356815</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A68" s="1">
         <v>41974</v>
       </c>
@@ -1879,7 +1879,7 @@
         <v>0.37778068364333517</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A69" s="1">
         <v>42005</v>
       </c>
@@ -1900,7 +1900,7 @@
         <v>0.7030492025674604</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A70" s="1">
         <v>42036</v>
       </c>
@@ -1921,7 +1921,7 @@
         <v>3.0589841511884557</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A71" s="1">
         <v>42064</v>
       </c>
@@ -1942,7 +1942,7 @@
         <v>-7.2345328442443302</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A72" s="1">
         <v>42095</v>
       </c>
@@ -1963,7 +1963,7 @@
         <v>4.0194708799602541</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A73" s="1">
         <v>42125</v>
       </c>
@@ -1984,7 +1984,7 @@
         <v>4.703991421736812</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A74" s="1">
         <v>42156</v>
       </c>
@@ -2005,7 +2005,7 @@
         <v>0.21046919582843396</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A75" s="1">
         <v>42186</v>
       </c>
@@ -2026,7 +2026,7 @@
         <v>3.3995079115904341</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A76" s="1">
         <v>42217</v>
       </c>
@@ -2047,7 +2047,7 @@
         <v>4.3382142435748889</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A77" s="1">
         <v>42248</v>
       </c>
@@ -2068,7 +2068,7 @@
         <v>0.20338165761323504</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A78" s="1">
         <v>42278</v>
       </c>
@@ -2089,7 +2089,7 @@
         <v>3.1908735463174827</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A79" s="1">
         <v>42309</v>
       </c>
@@ -2110,7 +2110,7 @@
         <v>1.6905934941460108</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A80" s="1">
         <v>42339</v>
       </c>
@@ -2131,7 +2131,7 @@
         <v>-2.3097839112622185</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A81" s="1">
         <v>42370</v>
       </c>
@@ -2152,7 +2152,7 @@
         <v>-18.926246340328831</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A82" s="1">
         <v>42401</v>
       </c>
@@ -2173,7 +2173,7 @@
         <v>-27.844964411669164</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A83" s="1">
         <v>42430</v>
       </c>
@@ -2194,7 +2194,7 @@
         <v>-4.5117101213726984</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A84" s="1">
         <v>42461</v>
       </c>
@@ -2215,7 +2215,7 @@
         <v>14.22663694809731</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A85" s="1">
         <v>42491</v>
       </c>
@@ -2236,7 +2236,7 @@
         <v>4.6207137961045417</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A86" s="1">
         <v>42522</v>
       </c>
@@ -2257,7 +2257,7 @@
         <v>-5.7394069639876264</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A87" s="1">
         <v>42552</v>
       </c>
@@ -2278,7 +2278,7 @@
         <v>-18.571671138659291</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A88" s="1">
         <v>42583</v>
       </c>
@@ -2299,7 +2299,7 @@
         <v>1.5296065663663629</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A89" s="1">
         <v>42614</v>
       </c>
@@ -2320,7 +2320,7 @@
         <v>-7.8739959707377407</v>
       </c>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A90" s="1">
         <v>42644</v>
       </c>
@@ -2341,7 +2341,7 @@
         <v>27.632202208103124</v>
       </c>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A91" s="1">
         <v>42675</v>
       </c>
@@ -2362,7 +2362,7 @@
         <v>-0.86939955289655135</v>
       </c>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A92" s="1">
         <v>42705</v>
       </c>
@@ -2383,7 +2383,7 @@
         <v>-8.4954865128245718</v>
       </c>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A93" s="1">
         <v>42736</v>
       </c>
@@ -2404,7 +2404,7 @@
         <v>0.43705851865527107</v>
       </c>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A94" s="1">
         <v>42767</v>
       </c>
@@ -2425,7 +2425,7 @@
         <v>-2.1102852373900061</v>
       </c>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A95" s="1">
         <v>42795</v>
       </c>
@@ -2446,7 +2446,7 @@
         <v>-0.97854264988672179</v>
       </c>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A96" s="1">
         <v>42826</v>
       </c>
@@ -2467,7 +2467,7 @@
         <v>-7.3064906118370532</v>
       </c>
     </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A97" s="1">
         <v>42856</v>
       </c>
@@ -2488,7 +2488,7 @@
         <v>-1.2942372868053735</v>
       </c>
     </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A98" s="1">
         <v>42887</v>
       </c>
@@ -2509,7 +2509,7 @@
         <v>5.8547423289047336</v>
       </c>
     </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A99" s="1">
         <v>42917</v>
       </c>
@@ -2530,7 +2530,7 @@
         <v>6.0426090142270121</v>
       </c>
     </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A100" s="1">
         <v>42948</v>
       </c>
@@ -2551,7 +2551,7 @@
         <v>7.0615559966585337</v>
       </c>
     </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A101" s="1">
         <v>42979</v>
       </c>
@@ -2572,7 +2572,7 @@
         <v>18.399003908887281</v>
       </c>
     </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A102" s="1">
         <v>43009</v>
       </c>
@@ -2593,7 +2593,7 @@
         <v>6.5660880262194601</v>
       </c>
     </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A103" s="1">
         <v>43040</v>
       </c>
@@ -2614,7 +2614,7 @@
         <v>4.0786728822630867</v>
       </c>
     </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A104" s="1">
         <v>43070</v>
       </c>
@@ -2635,7 +2635,7 @@
         <v>-0.93815024599723607</v>
       </c>
     </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A105" s="1">
         <v>43101</v>
       </c>
@@ -2656,7 +2656,7 @@
         <v>10.08798583318085</v>
       </c>
     </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A106" s="1">
         <v>43132</v>
       </c>
@@ -2677,7 +2677,7 @@
         <v>12.601443695256464</v>
       </c>
     </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A107" s="1">
         <v>43160</v>
       </c>
@@ -2698,7 +2698,7 @@
         <v>19.522893789328162</v>
       </c>
     </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A108" s="1">
         <v>43191</v>
       </c>
@@ -2719,7 +2719,7 @@
         <v>14.540961442002962</v>
       </c>
     </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A109" s="1">
         <v>43221</v>
       </c>
@@ -2740,7 +2740,7 @@
         <v>10.475795085170155</v>
       </c>
     </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A110" s="1">
         <v>43252</v>
       </c>
@@ -2761,7 +2761,7 @@
         <v>2.0510121997912507</v>
       </c>
     </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A111" s="1">
         <v>43282</v>
       </c>
@@ -2782,7 +2782,7 @@
         <v>7.8351861344362757</v>
       </c>
     </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A112" s="1">
         <v>43313</v>
       </c>
@@ -2803,7 +2803,7 @@
         <v>14.23900818825372</v>
       </c>
     </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A113" s="1">
         <v>43344</v>
       </c>
@@ -2824,7 +2824,7 @@
         <v>12.105593238208256</v>
       </c>
     </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A114" s="1">
         <v>43374</v>
       </c>
@@ -2845,7 +2845,7 @@
         <v>-9.4104144237393292</v>
       </c>
     </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A115" s="1">
         <v>43405</v>
       </c>
@@ -2866,7 +2866,7 @@
         <v>-1.4379612130621116</v>
       </c>
     </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A116" s="1">
         <v>43435</v>
       </c>
@@ -2887,7 +2887,7 @@
         <v>14.897205611904333</v>
       </c>
     </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A117" s="1">
         <v>43466</v>
       </c>
@@ -2908,7 +2908,7 @@
         <v>3.6298259634816308</v>
       </c>
     </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A118" s="1">
         <v>43497</v>
       </c>
@@ -2929,7 +2929,7 @@
         <v>-10.676960325376955</v>
       </c>
     </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A119" s="1">
         <v>43525</v>
       </c>
@@ -2950,7 +2950,7 @@
         <v>4.0642216274141978</v>
       </c>
     </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A120" s="1">
         <v>43556</v>
       </c>
@@ -2971,7 +2971,7 @@
         <v>15.421970662647185</v>
       </c>
     </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A121" s="1">
         <v>43586</v>
       </c>
@@ -2992,7 +2992,7 @@
         <v>-0.35986066625680985</v>
       </c>
     </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A122" s="1">
         <v>43617</v>
       </c>
@@ -3013,7 +3013,7 @@
         <v>-1.0777569709117947</v>
       </c>
     </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A123" s="1">
         <v>43647</v>
       </c>
@@ -3034,7 +3034,7 @@
         <v>10.466822637701094</v>
       </c>
     </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A124" s="1">
         <v>43678</v>
       </c>
@@ -3055,7 +3055,7 @@
         <v>-3.8091768216451536</v>
       </c>
     </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A125" s="1">
         <v>43709</v>
       </c>
@@ -3076,7 +3076,7 @@
         <v>-4.750736678601438</v>
       </c>
     </row>
-    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A126" s="1">
         <v>43739</v>
       </c>
@@ -3097,7 +3097,7 @@
         <v>-4.7537808762193521</v>
       </c>
     </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A127" s="1">
         <v>43770</v>
       </c>
@@ -3118,7 +3118,7 @@
         <v>-0.8943330033649185</v>
       </c>
     </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A128" s="1">
         <v>43800</v>
       </c>
@@ -3139,10 +3139,10 @@
         <v>2.3499313001612356</v>
       </c>
     </row>
-    <row r="130" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="130" spans="5:5" x14ac:dyDescent="0.35">
       <c r="E130" s="2"/>
     </row>
-    <row r="131" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="131" spans="5:5" x14ac:dyDescent="0.35">
       <c r="E131" s="2"/>
     </row>
   </sheetData>

</xml_diff>